<commit_message>
Release 0.0.0 - Finish script
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\Personal Projects\Python-WhatsApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962D0E6D-A147-4992-8A80-987CF205B22F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90C220F-6C9E-4C1C-A02A-28666278EC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3585" yWindow="3585" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,8 +24,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Sergio Gutiérrez Sanchez</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{599AF722-E0EC-43BE-9F0F-F6EE1DB1330B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Sergio Gutiérrez Sanchez:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+Mantener en Tipo Texto</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>Nombre</t>
   </si>
@@ -39,10 +71,25 @@
     <t>Imagen</t>
   </si>
   <si>
-    <t>User 1</t>
-  </si>
-  <si>
-    <t>User 2</t>
+    <t>User1</t>
+  </si>
+  <si>
+    <t>+51xxxxxxxxx</t>
+  </si>
+  <si>
+    <t>text1</t>
+  </si>
+  <si>
+    <t>User2</t>
+  </si>
+  <si>
+    <t>text2</t>
+  </si>
+  <si>
+    <t>text3</t>
+  </si>
+  <si>
+    <t>robot_hi.png</t>
   </si>
 </sst>
 </file>
@@ -52,7 +99,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +121,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
     </font>
   </fonts>
   <fills count="2">
@@ -106,13 +164,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -393,14 +455,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -420,36 +488,63 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="C3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
+      <c r="B5" s="6"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
+      <c r="B6" s="6"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
+      <c r="B7" s="6"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
+      <c r="B8" s="6"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="1"/>
+      <c r="B9" s="6"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="1"/>
+      <c r="B10" s="6"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
@@ -701,5 +796,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>